<commit_message>
Reading of the input file is not finished yet.
</commit_message>
<xml_diff>
--- a/doc/game001.xlsx
+++ b/doc/game001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -92,6 +92,9 @@
     <t xml:space="preserve">FRUIT06</t>
   </si>
   <si>
+    <t xml:space="preserve">FRUIT07</t>
+  </si>
+  <si>
     <t xml:space="preserve">Symbol \ Length</t>
   </si>
   <si>
@@ -111,9 +114,6 @@
   </si>
   <si>
     <t xml:space="preserve">0 of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRUIT07</t>
   </si>
   <si>
     <t xml:space="preserve">О</t>
@@ -126,9 +126,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -195,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,8 +205,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -233,9 +238,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,15 +317,14 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,7 +401,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>16</v>
@@ -427,31 +431,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +643,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>100</v>
@@ -679,14 +682,13 @@
   </sheetPr>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="2" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="2" width="2.02551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,11 +743,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -799,11 +801,11 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -857,11 +859,11 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
@@ -915,11 +917,11 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
@@ -973,11 +975,11 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -1031,11 +1033,11 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -1089,11 +1091,11 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -1147,11 +1149,11 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1205,11 +1207,11 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0"/>
-      <c r="C36" s="0"/>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
@@ -1263,11 +1265,11 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
@@ -1321,11 +1323,11 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="D44" s="0"/>
-      <c r="E44" s="0"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
@@ -1379,11 +1381,11 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0"/>
-      <c r="B48" s="0"/>
-      <c r="C48" s="0"/>
-      <c r="D48" s="0"/>
-      <c r="E48" s="0"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
@@ -1437,11 +1439,11 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
-      <c r="B52" s="0"/>
-      <c r="C52" s="0"/>
-      <c r="D52" s="0"/>
-      <c r="E52" s="0"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
@@ -1495,11 +1497,11 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
-      <c r="D56" s="0"/>
-      <c r="E56" s="0"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
@@ -1553,11 +1555,11 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0"/>
-      <c r="B60" s="0"/>
-      <c r="C60" s="0"/>
-      <c r="D60" s="0"/>
-      <c r="E60" s="0"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
@@ -1611,11 +1613,11 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0"/>
-      <c r="B64" s="0"/>
-      <c r="C64" s="0"/>
-      <c r="D64" s="0"/>
-      <c r="E64" s="0"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
@@ -1669,11 +1671,11 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="0"/>
-      <c r="C68" s="0"/>
-      <c r="D68" s="0"/>
-      <c r="E68" s="0"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
@@ -1727,11 +1729,11 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0"/>
-      <c r="B72" s="0"/>
-      <c r="C72" s="0"/>
-      <c r="D72" s="0"/>
-      <c r="E72" s="0"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
@@ -1785,11 +1787,11 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0"/>
-      <c r="B76" s="0"/>
-      <c r="C76" s="0"/>
-      <c r="D76" s="0"/>
-      <c r="E76" s="0"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
@@ -1860,14 +1862,11 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2007,19 +2006,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reading of the input file was done.
</commit_message>
<xml_diff>
--- a/doc/game001.xlsx
+++ b/doc/game001.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Symbols" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Paytable" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Lines" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Reels 95.5 RTP" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Base Reels 95.5 RTP" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Free Reels 95.5 RTP" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -238,9 +239,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,14 +317,15 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,7 +432,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,7 +690,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="2" width="2.02551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="2" width="1.88775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,11 +1865,14 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2030,4 +2036,30 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial reels generation was done.
</commit_message>
<xml_diff>
--- a/doc/game001.xlsx
+++ b/doc/game001.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="32">
   <si>
     <t xml:space="preserve">Game Title</t>
   </si>
@@ -239,8 +239,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,9 +324,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,8 +433,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,8 +691,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="2" width="1.88775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="2" width="1.75510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,15 +1864,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,120 +1911,1157 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2051,7 +3089,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>